<commit_message>
xong manage Doctor profile
</commit_message>
<xml_diff>
--- a/back-end/fileDataDB/allcode.xlsx
+++ b/back-end/fileDataDB/allcode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HealthBooking\back-end\fileDataDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE7A270-5D79-41C9-8AF7-23E0605A7F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B7435EB-0B1A-4225-BA2D-C0D1A5C5EE1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{B89DABE2-1255-4D9D-9660-33C35DF0348B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="207">
   <si>
     <t>type</t>
   </si>
@@ -104,9 +104,6 @@
     <t>POSITION</t>
   </si>
   <si>
-    <t>P0</t>
-  </si>
-  <si>
     <t>P1</t>
   </si>
   <si>
@@ -200,30 +197,6 @@
     <t>Đã hủy</t>
   </si>
   <si>
-    <t>8:00 - 9:00</t>
-  </si>
-  <si>
-    <t>9:00 - 10:00</t>
-  </si>
-  <si>
-    <t>10:00 - 11:00</t>
-  </si>
-  <si>
-    <t>11:00 - 12:00</t>
-  </si>
-  <si>
-    <t>13:00 - 14:00</t>
-  </si>
-  <si>
-    <t>14:00 - 15:00</t>
-  </si>
-  <si>
-    <t>15:00 - 16:00</t>
-  </si>
-  <si>
-    <t>16:00 - 17:00</t>
-  </si>
-  <si>
     <t>Thạc sĩ</t>
   </si>
   <si>
@@ -257,9 +230,6 @@
     <t>Hà Nội</t>
   </si>
   <si>
-    <t>Hồ Chí Minh</t>
-  </si>
-  <si>
     <t>Đà Nẵng</t>
   </si>
   <si>
@@ -284,18 +254,12 @@
     <t>Khánh Hòa</t>
   </si>
   <si>
-    <t>7:00-8:00</t>
-  </si>
-  <si>
     <t>T9</t>
   </si>
   <si>
     <t>T10</t>
   </si>
   <si>
-    <t>17:00-18:00</t>
-  </si>
-  <si>
     <t>PR1</t>
   </si>
   <si>
@@ -321,6 +285,378 @@
   </si>
   <si>
     <t>PR9</t>
+  </si>
+  <si>
+    <t>7:00 - 7:30</t>
+  </si>
+  <si>
+    <t>7:30 - 8:00</t>
+  </si>
+  <si>
+    <t>8:30 - 9:00</t>
+  </si>
+  <si>
+    <t>9:30 - 10:00</t>
+  </si>
+  <si>
+    <t>10:30 - 11:00</t>
+  </si>
+  <si>
+    <t>11:00 - 11:30</t>
+  </si>
+  <si>
+    <t>13:00 - 13:30</t>
+  </si>
+  <si>
+    <t>13:30 -14:00</t>
+  </si>
+  <si>
+    <t>14:00 - 14:30</t>
+  </si>
+  <si>
+    <t>15:00 - 15:30</t>
+  </si>
+  <si>
+    <t>T11</t>
+  </si>
+  <si>
+    <t>15:30 - 16:00</t>
+  </si>
+  <si>
+    <t>T12</t>
+  </si>
+  <si>
+    <t>T13</t>
+  </si>
+  <si>
+    <t>16:00 - 16:30</t>
+  </si>
+  <si>
+    <t>16:30 - 17:00</t>
+  </si>
+  <si>
+    <t>Hòa Bình</t>
+  </si>
+  <si>
+    <t>Sơn La</t>
+  </si>
+  <si>
+    <t>Điện Biên</t>
+  </si>
+  <si>
+    <t>Lai Châu</t>
+  </si>
+  <si>
+    <t>Lào Cai</t>
+  </si>
+  <si>
+    <t>Yên Bái</t>
+  </si>
+  <si>
+    <t>Phú Thọ</t>
+  </si>
+  <si>
+    <t>Hà Giang</t>
+  </si>
+  <si>
+    <t>Tuyên Quang</t>
+  </si>
+  <si>
+    <t>Cao Bằng</t>
+  </si>
+  <si>
+    <t>Bắc Kạn</t>
+  </si>
+  <si>
+    <t>Thái Nguyên</t>
+  </si>
+  <si>
+    <t>Lạng Sơn</t>
+  </si>
+  <si>
+    <t>Bắc Giang</t>
+  </si>
+  <si>
+    <t>Bắc Ninh</t>
+  </si>
+  <si>
+    <t>Hà Nam</t>
+  </si>
+  <si>
+    <t>Hải Dương</t>
+  </si>
+  <si>
+    <t>Hải Phòng</t>
+  </si>
+  <si>
+    <t>Hưng Yên</t>
+  </si>
+  <si>
+    <t>Nam Định</t>
+  </si>
+  <si>
+    <t>Thái Bình</t>
+  </si>
+  <si>
+    <t>Vĩnh Phúc</t>
+  </si>
+  <si>
+    <t>Ninh Bình</t>
+  </si>
+  <si>
+    <t>Thanh Hóa</t>
+  </si>
+  <si>
+    <t>Nghệ An</t>
+  </si>
+  <si>
+    <t>Hà Tĩnh</t>
+  </si>
+  <si>
+    <t>Quảng Trị</t>
+  </si>
+  <si>
+    <t>Quảng Nam</t>
+  </si>
+  <si>
+    <t>Quảng Ngãi</t>
+  </si>
+  <si>
+    <t>Bình Định</t>
+  </si>
+  <si>
+    <t>Phú Yên</t>
+  </si>
+  <si>
+    <t>Ninh Thuận</t>
+  </si>
+  <si>
+    <t>Bình Thuận</t>
+  </si>
+  <si>
+    <t>Kon Tum</t>
+  </si>
+  <si>
+    <t>Gia Lai</t>
+  </si>
+  <si>
+    <t>Đắk Lắk</t>
+  </si>
+  <si>
+    <t>Đắk Nông</t>
+  </si>
+  <si>
+    <t>Lâm Đồng</t>
+  </si>
+  <si>
+    <t>TP Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>Bà Rịa Vũng Tàu</t>
+  </si>
+  <si>
+    <t>Bình Phước</t>
+  </si>
+  <si>
+    <t>Tây Ninh</t>
+  </si>
+  <si>
+    <t>An Giang</t>
+  </si>
+  <si>
+    <t>Bạc Liêu</t>
+  </si>
+  <si>
+    <t>Bến Tre</t>
+  </si>
+  <si>
+    <t>Cà Mau</t>
+  </si>
+  <si>
+    <t>Đồng Tháp</t>
+  </si>
+  <si>
+    <t>Hậu Giang</t>
+  </si>
+  <si>
+    <t>Kiên Giang</t>
+  </si>
+  <si>
+    <t>Long An</t>
+  </si>
+  <si>
+    <t>Sóc Trăng</t>
+  </si>
+  <si>
+    <t>Tiền Giang</t>
+  </si>
+  <si>
+    <t>Trà Vinh</t>
+  </si>
+  <si>
+    <t>Vĩnh Long</t>
+  </si>
+  <si>
+    <t>PRO11</t>
+  </si>
+  <si>
+    <t>PRO12</t>
+  </si>
+  <si>
+    <t>PRO13</t>
+  </si>
+  <si>
+    <t>PRO14</t>
+  </si>
+  <si>
+    <t>PRO15</t>
+  </si>
+  <si>
+    <t>PRO16</t>
+  </si>
+  <si>
+    <t>PRO17</t>
+  </si>
+  <si>
+    <t>PRO18</t>
+  </si>
+  <si>
+    <t>PRO19</t>
+  </si>
+  <si>
+    <t>PRO20</t>
+  </si>
+  <si>
+    <t>PRO21</t>
+  </si>
+  <si>
+    <t>PRO22</t>
+  </si>
+  <si>
+    <t>PRO23</t>
+  </si>
+  <si>
+    <t>PRO24</t>
+  </si>
+  <si>
+    <t>PRO25</t>
+  </si>
+  <si>
+    <t>PRO26</t>
+  </si>
+  <si>
+    <t>PRO27</t>
+  </si>
+  <si>
+    <t>PRO28</t>
+  </si>
+  <si>
+    <t>PRO29</t>
+  </si>
+  <si>
+    <t>PRO30</t>
+  </si>
+  <si>
+    <t>PRO31</t>
+  </si>
+  <si>
+    <t>PRO32</t>
+  </si>
+  <si>
+    <t>PRO33</t>
+  </si>
+  <si>
+    <t>PRO34</t>
+  </si>
+  <si>
+    <t>PRO35</t>
+  </si>
+  <si>
+    <t>PRO36</t>
+  </si>
+  <si>
+    <t>PRO37</t>
+  </si>
+  <si>
+    <t>PRO38</t>
+  </si>
+  <si>
+    <t>PRO39</t>
+  </si>
+  <si>
+    <t>PRO40</t>
+  </si>
+  <si>
+    <t>PRO41</t>
+  </si>
+  <si>
+    <t>PRO42</t>
+  </si>
+  <si>
+    <t>PRO43</t>
+  </si>
+  <si>
+    <t>PRO44</t>
+  </si>
+  <si>
+    <t>PRO45</t>
+  </si>
+  <si>
+    <t>PRO46</t>
+  </si>
+  <si>
+    <t>PRO47</t>
+  </si>
+  <si>
+    <t>PRO48</t>
+  </si>
+  <si>
+    <t>PRO49</t>
+  </si>
+  <si>
+    <t>PRO50</t>
+  </si>
+  <si>
+    <t>PRO51</t>
+  </si>
+  <si>
+    <t>PRO52</t>
+  </si>
+  <si>
+    <t>PRO53</t>
+  </si>
+  <si>
+    <t>PRO54</t>
+  </si>
+  <si>
+    <t>PRO55</t>
+  </si>
+  <si>
+    <t>PRO56</t>
+  </si>
+  <si>
+    <t>PRO57</t>
+  </si>
+  <si>
+    <t>PRO58</t>
+  </si>
+  <si>
+    <t>PRO59</t>
+  </si>
+  <si>
+    <t>PRO60</t>
+  </si>
+  <si>
+    <t>PRO61</t>
+  </si>
+  <si>
+    <t>PRO62</t>
+  </si>
+  <si>
+    <t>PRO63</t>
+  </si>
+  <si>
+    <t>P5</t>
   </si>
 </sst>
 </file>
@@ -356,7 +692,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -379,17 +715,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -705,10 +1065,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DA6D3AE-A9F9-4B72-9B6C-41CF6E4EA0C0}">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:D104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,7 +1089,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -737,7 +1097,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -748,10 +1108,10 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -759,10 +1119,10 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -770,10 +1130,10 @@
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -781,10 +1141,10 @@
         <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -792,7 +1152,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -803,7 +1163,7 @@
         <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -814,10 +1174,10 @@
         <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -825,10 +1185,10 @@
         <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -836,10 +1196,10 @@
         <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -847,10 +1207,10 @@
         <v>16</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -858,10 +1218,10 @@
         <v>17</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -869,10 +1229,10 @@
         <v>18</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -880,10 +1240,10 @@
         <v>19</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -891,73 +1251,73 @@
         <v>20</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>22</v>
+        <v>93</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>48</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>23</v>
+        <v>95</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>62</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>24</v>
+        <v>96</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -965,289 +1325,965 @@
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>30</v>
+        <v>206</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C27" s="1">
-        <v>100000</v>
+        <v>27</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C28" s="1">
-        <v>150000</v>
+        <v>28</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C29" s="1">
-        <v>200000</v>
+        <v>29</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="C30" s="1">
-        <v>250000</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="C31" s="1">
-        <v>300000</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" s="1">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C33" s="1">
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" s="1">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" s="1">
+        <v>350000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C36" s="1">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C37" s="1">
+        <v>450000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38" s="1">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C32" s="1">
-        <v>350000</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
+      <c r="B39" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C33" s="1">
-        <v>400000</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
+      <c r="B40" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C34" s="1">
-        <v>450000</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C35" s="1">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C36" s="1" t="s">
+      <c r="B41" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D42" s="2"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D43" s="2"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D44" s="2"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D45" s="2"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D46" s="2"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D47" s="2"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D48" s="2"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D49" s="2"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D50" s="2"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D51" s="2"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D52" s="2"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D53" s="2"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D54" s="2"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D55" s="2"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D56" s="2"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D57" s="2"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D58" s="2"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D59" s="2"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D60" s="2"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D61" s="2"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D62" s="2"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D63" s="2"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D64" s="2"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D65" s="2"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D66" s="2"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D67" s="2"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D68" s="2"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D69" s="2"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D70" s="2"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D71" s="2"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C72" s="4" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C38" s="1" t="s">
+      <c r="D72" s="2"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D73" s="2"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D74" s="2"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D75" s="2"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D76" s="2"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D77" s="2"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C78" s="4" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="49" spans="3:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C49" s="2"/>
+      <c r="D78" s="2"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D79" s="2"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D80" s="2"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D81" s="2"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D82" s="2"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D83" s="2"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D84" s="2"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D85" s="2"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D86" s="2"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D87" s="2"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D88" s="2"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D89" s="2"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D90" s="2"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D91" s="2"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D92" s="2"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D93" s="2"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D94" s="2"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D95" s="2"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D96" s="2"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D97" s="2"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C98" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D98" s="2"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D99" s="2"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C100" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D100" s="2"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C101" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D101" s="2"/>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C102" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D102" s="2"/>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C103" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D103" s="2"/>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C104" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D104" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
load xong schedule, datepickre
</commit_message>
<xml_diff>
--- a/back-end/fileDataDB/allcode.xlsx
+++ b/back-end/fileDataDB/allcode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HealthBooking\back-end\fileDataDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B7435EB-0B1A-4225-BA2D-C0D1A5C5EE1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5144D692-A65C-49CD-BFC2-B7791708455C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{B89DABE2-1255-4D9D-9660-33C35DF0348B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="215">
   <si>
     <t>type</t>
   </si>
@@ -657,6 +657,30 @@
   </si>
   <si>
     <t>P5</t>
+  </si>
+  <si>
+    <t>8:00 - 8:30</t>
+  </si>
+  <si>
+    <t>9:00 - 9:30</t>
+  </si>
+  <si>
+    <t>10:00 - 10:30</t>
+  </si>
+  <si>
+    <t>14:30 - 15:00</t>
+  </si>
+  <si>
+    <t>T14</t>
+  </si>
+  <si>
+    <t>T15</t>
+  </si>
+  <si>
+    <t>T16</t>
+  </si>
+  <si>
+    <t>T17</t>
   </si>
 </sst>
 </file>
@@ -1065,10 +1089,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DA6D3AE-A9F9-4B72-9B6C-41CF6E4EA0C0}">
-  <dimension ref="A1:D104"/>
+  <dimension ref="A1:D108"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1196,7 +1220,7 @@
         <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>85</v>
+        <v>207</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1207,7 +1231,7 @@
         <v>16</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1218,7 +1242,7 @@
         <v>17</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>87</v>
+        <v>208</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1229,7 +1253,7 @@
         <v>18</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1240,7 +1264,7 @@
         <v>19</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>89</v>
+        <v>209</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1251,7 +1275,7 @@
         <v>20</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1262,7 +1286,7 @@
         <v>72</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1273,7 +1297,7 @@
         <v>73</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1284,7 +1308,7 @@
         <v>93</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1295,7 +1319,7 @@
         <v>95</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1306,51 +1330,51 @@
         <v>96</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>98</v>
+        <v>210</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>22</v>
+        <v>211</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>23</v>
+        <v>212</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>53</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>24</v>
+        <v>213</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>54</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>25</v>
+        <v>214</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>55</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1358,87 +1382,87 @@
         <v>21</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>206</v>
+        <v>22</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C30" s="1">
-        <v>100000</v>
+        <v>206</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C31" s="1">
-        <v>150000</v>
+        <v>27</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C32" s="1">
-        <v>200000</v>
+        <v>28</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C33" s="1">
-        <v>250000</v>
+        <v>29</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1446,10 +1470,10 @@
         <v>30</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C34" s="1">
-        <v>300000</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1457,10 +1481,10 @@
         <v>30</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C35" s="1">
-        <v>350000</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1468,10 +1492,10 @@
         <v>30</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C36" s="1">
-        <v>400000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1479,10 +1503,10 @@
         <v>30</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C37" s="1">
-        <v>450000</v>
+        <v>250000</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1490,102 +1514,98 @@
         <v>30</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C38" s="1">
-        <v>500000</v>
+        <v>300000</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>60</v>
+        <v>79</v>
+      </c>
+      <c r="C39" s="1">
+        <v>350000</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>61</v>
+        <v>80</v>
+      </c>
+      <c r="C40" s="1">
+        <v>400000</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C41" s="1">
+        <v>450000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C42" s="1">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B43" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D42" s="2"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D43" s="2"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D44" s="2"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D45" s="2"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D46" s="2"/>
     </row>
@@ -1594,10 +1614,10 @@
         <v>35</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D47" s="2"/>
     </row>
@@ -1606,10 +1626,10 @@
         <v>35</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D48" s="2"/>
     </row>
@@ -1618,10 +1638,10 @@
         <v>35</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D49" s="2"/>
     </row>
@@ -1630,10 +1650,10 @@
         <v>35</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D50" s="2"/>
     </row>
@@ -1642,10 +1662,10 @@
         <v>35</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D51" s="2"/>
     </row>
@@ -1654,10 +1674,10 @@
         <v>35</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>153</v>
+        <v>42</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D52" s="2"/>
     </row>
@@ -1666,10 +1686,10 @@
         <v>35</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>154</v>
+        <v>43</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D53" s="2"/>
     </row>
@@ -1678,10 +1698,10 @@
         <v>35</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>155</v>
+        <v>44</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D54" s="2"/>
     </row>
@@ -1690,10 +1710,10 @@
         <v>35</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>156</v>
+        <v>45</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D55" s="2"/>
     </row>
@@ -1702,10 +1722,10 @@
         <v>35</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>68</v>
+        <v>109</v>
       </c>
       <c r="D56" s="2"/>
     </row>
@@ -1714,10 +1734,10 @@
         <v>35</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>63</v>
+        <v>110</v>
       </c>
       <c r="D57" s="2"/>
     </row>
@@ -1726,10 +1746,10 @@
         <v>35</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D58" s="2"/>
     </row>
@@ -1738,10 +1758,10 @@
         <v>35</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D59" s="2"/>
     </row>
@@ -1750,10 +1770,10 @@
         <v>35</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>115</v>
+        <v>68</v>
       </c>
       <c r="D60" s="2"/>
     </row>
@@ -1762,10 +1782,10 @@
         <v>35</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>116</v>
+        <v>63</v>
       </c>
       <c r="D61" s="2"/>
     </row>
@@ -1774,10 +1794,10 @@
         <v>35</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D62" s="2"/>
     </row>
@@ -1786,10 +1806,10 @@
         <v>35</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D63" s="2"/>
     </row>
@@ -1798,10 +1818,10 @@
         <v>35</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D64" s="2"/>
     </row>
@@ -1810,10 +1830,10 @@
         <v>35</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D65" s="2"/>
     </row>
@@ -1822,10 +1842,10 @@
         <v>35</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>121</v>
+        <v>163</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="D66" s="2"/>
     </row>
@@ -1834,10 +1854,10 @@
         <v>35</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>122</v>
+        <v>164</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="D67" s="2"/>
     </row>
@@ -1846,10 +1866,10 @@
         <v>35</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>123</v>
+        <v>165</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>119</v>
       </c>
       <c r="D68" s="2"/>
     </row>
@@ -1858,10 +1878,10 @@
         <v>35</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>124</v>
+        <v>166</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="D69" s="2"/>
     </row>
@@ -1870,10 +1890,10 @@
         <v>35</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>70</v>
+        <v>167</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="D70" s="2"/>
     </row>
@@ -1882,10 +1902,10 @@
         <v>35</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D71" s="2"/>
     </row>
@@ -1894,10 +1914,10 @@
         <v>35</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>69</v>
+        <v>123</v>
       </c>
       <c r="D72" s="2"/>
     </row>
@@ -1906,10 +1926,10 @@
         <v>35</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>64</v>
+        <v>124</v>
       </c>
       <c r="D73" s="2"/>
     </row>
@@ -1918,10 +1938,10 @@
         <v>35</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>126</v>
+        <v>70</v>
       </c>
       <c r="D74" s="2"/>
     </row>
@@ -1930,10 +1950,10 @@
         <v>35</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D75" s="2"/>
     </row>
@@ -1942,10 +1962,10 @@
         <v>35</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>128</v>
+        <v>69</v>
       </c>
       <c r="D76" s="2"/>
     </row>
@@ -1954,10 +1974,10 @@
         <v>35</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>129</v>
+        <v>64</v>
       </c>
       <c r="D77" s="2"/>
     </row>
@@ -1966,10 +1986,10 @@
         <v>35</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>71</v>
+        <v>126</v>
       </c>
       <c r="D78" s="2"/>
     </row>
@@ -1978,10 +1998,10 @@
         <v>35</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D79" s="2"/>
     </row>
@@ -1990,10 +2010,10 @@
         <v>35</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D80" s="2"/>
     </row>
@@ -2002,10 +2022,10 @@
         <v>35</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D81" s="2"/>
     </row>
@@ -2014,10 +2034,10 @@
         <v>35</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>133</v>
+        <v>71</v>
       </c>
       <c r="D82" s="2"/>
     </row>
@@ -2026,10 +2046,10 @@
         <v>35</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D83" s="2"/>
     </row>
@@ -2038,10 +2058,10 @@
         <v>35</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D84" s="2"/>
     </row>
@@ -2050,10 +2070,10 @@
         <v>35</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D85" s="2"/>
     </row>
@@ -2062,10 +2082,10 @@
         <v>35</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D86" s="2"/>
     </row>
@@ -2074,10 +2094,10 @@
         <v>35</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D87" s="2"/>
     </row>
@@ -2086,10 +2106,10 @@
         <v>35</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>66</v>
+        <v>135</v>
       </c>
       <c r="D88" s="2"/>
     </row>
@@ -2098,10 +2118,10 @@
         <v>35</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D89" s="2"/>
     </row>
@@ -2110,10 +2130,10 @@
         <v>35</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>67</v>
+        <v>137</v>
       </c>
       <c r="D90" s="2"/>
     </row>
@@ -2122,10 +2142,10 @@
         <v>35</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D91" s="2"/>
     </row>
@@ -2134,10 +2154,10 @@
         <v>35</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>141</v>
+        <v>66</v>
       </c>
       <c r="D92" s="2"/>
     </row>
@@ -2146,10 +2166,10 @@
         <v>35</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D93" s="2"/>
     </row>
@@ -2158,10 +2178,10 @@
         <v>35</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>143</v>
+        <v>67</v>
       </c>
       <c r="D94" s="2"/>
     </row>
@@ -2170,10 +2190,10 @@
         <v>35</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D95" s="2"/>
     </row>
@@ -2182,10 +2202,10 @@
         <v>35</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>65</v>
+        <v>141</v>
       </c>
       <c r="D96" s="2"/>
     </row>
@@ -2194,10 +2214,10 @@
         <v>35</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D97" s="2"/>
     </row>
@@ -2206,10 +2226,10 @@
         <v>35</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D98" s="2"/>
     </row>
@@ -2218,10 +2238,10 @@
         <v>35</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D99" s="2"/>
     </row>
@@ -2230,10 +2250,10 @@
         <v>35</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>148</v>
+        <v>65</v>
       </c>
       <c r="D100" s="2"/>
     </row>
@@ -2242,10 +2262,10 @@
         <v>35</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D101" s="2"/>
     </row>
@@ -2254,10 +2274,10 @@
         <v>35</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D102" s="2"/>
     </row>
@@ -2266,10 +2286,10 @@
         <v>35</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D103" s="2"/>
     </row>
@@ -2278,12 +2298,60 @@
         <v>35</v>
       </c>
       <c r="B104" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C104" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D104" s="2"/>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C105" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D105" s="2"/>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C106" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D106" s="2"/>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C107" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D107" s="2"/>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B108" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="C104" s="4" t="s">
+      <c r="C108" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="D104" s="2"/>
+      <c r="D108" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>